<commit_message>
Fix errori segnalati 2024-05-02
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#BRAINCOMPUTINGXX/Brain Computing S.p.a/ReMed/2.0.1/report-checklist.xlsx
+++ b/GATEWAY/A1#111#BRAINCOMPUTINGXX/Brain Computing S.p.a/ReMed/2.0.1/report-checklist.xlsx
@@ -685,10 +685,10 @@
 </t>
   </si>
   <si>
-    <t>29/04/2024</t>
-  </si>
-  <si>
-    <t>2024-04-29T14:23:44+02:00</t>
+    <t>06/05/2024</t>
+  </si>
+  <si>
+    <t>2024-05-06T09:22:12+02:00</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT3</t>
@@ -700,7 +700,7 @@
 </t>
   </si>
   <si>
-    <t>2024-04-29T14:23:49+02:00</t>
+    <t>2024-05-06T09:22:16+02:00</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT4</t>
@@ -712,7 +712,7 @@
 </t>
   </si>
   <si>
-    <t>2024-04-29T14:23:53+02:00</t>
+    <t>2024-05-06T09:22:19+02:00</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT5_KO</t>

</xml_diff>

<commit_message>
Fix errori segnalati 2024-05-02 (ok)
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#BRAINCOMPUTINGXX/Brain Computing S.p.a/ReMed/2.0.1/report-checklist.xlsx
+++ b/GATEWAY/A1#111#BRAINCOMPUTINGXX/Brain Computing S.p.a/ReMed/2.0.1/report-checklist.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="679">
   <si>
     <t>NOME FORNITORE:</t>
   </si>
@@ -688,7 +688,13 @@
     <t>06/05/2024</t>
   </si>
   <si>
-    <t>2024-05-06T09:22:12+02:00</t>
+    <t>2024-05-06T09:43:46+02:00</t>
+  </si>
+  <si>
+    <t>f5c995f320bde7d0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.4042fcc253^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT3</t>
@@ -700,7 +706,13 @@
 </t>
   </si>
   <si>
-    <t>2024-05-06T09:22:16+02:00</t>
+    <t>2024-05-06T09:43:50+02:00</t>
+  </si>
+  <si>
+    <t>7fae384a4b44739e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.7ec121f9d6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT4</t>
@@ -712,7 +724,13 @@
 </t>
   </si>
   <si>
-    <t>2024-05-06T09:22:19+02:00</t>
+    <t>2024-05-06T09:43:55+02:00</t>
+  </si>
+  <si>
+    <t>394d0800bee224fe</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.f3c67ed423^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT5_KO</t>
@@ -4884,10 +4902,10 @@
         <v>152</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>32</v>
+        <v>153</v>
       </c>
       <c r="I36" s="15" t="s">
-        <v>33</v>
+        <v>154</v>
       </c>
       <c r="J36" s="16" t="s">
         <v>34</v>
@@ -4916,22 +4934,22 @@
         <v>63</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F37" s="14" t="s">
         <v>151</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>32</v>
+        <v>158</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>33</v>
+        <v>159</v>
       </c>
       <c r="J37" s="16" t="s">
         <v>34</v>
@@ -4960,22 +4978,22 @@
         <v>63</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="F38" s="14" t="s">
         <v>151</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>32</v>
+        <v>163</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>33</v>
+        <v>164</v>
       </c>
       <c r="J38" s="16" t="s">
         <v>34</v>
@@ -5004,22 +5022,22 @@
         <v>63</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="F39" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="I39" s="15" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="J39" s="16" t="s">
         <v>34</v>
@@ -5058,22 +5076,22 @@
         <v>63</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="F40" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G40" s="15" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="I40" s="15" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="J40" s="16" t="s">
         <v>34</v>
@@ -5112,22 +5130,22 @@
         <v>63</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="F41" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="I41" s="15" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="J41" s="16" t="s">
         <v>34</v>
@@ -5166,22 +5184,22 @@
         <v>63</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="F42" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="I42" s="15" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="J42" s="16" t="s">
         <v>34</v>
@@ -5220,22 +5238,22 @@
         <v>63</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="F43" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="I43" s="15" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="J43" s="16" t="s">
         <v>34</v>
@@ -5274,22 +5292,22 @@
         <v>63</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="F44" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G44" s="15" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="I44" s="15" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="J44" s="16" t="s">
         <v>34</v>
@@ -5328,22 +5346,22 @@
         <v>63</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="F45" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="H45" s="15" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="I45" s="15" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="J45" s="16" t="s">
         <v>34</v>
@@ -5382,22 +5400,22 @@
         <v>63</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="F46" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G46" s="15" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="H46" s="15" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="I46" s="15" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="J46" s="16" t="s">
         <v>34</v>
@@ -5436,22 +5454,22 @@
         <v>63</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F47" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="H47" s="15" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="I47" s="15" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="J47" s="16" t="s">
         <v>34</v>
@@ -5490,22 +5508,22 @@
         <v>63</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="F48" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G48" s="15" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="I48" s="15" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="J48" s="16" t="s">
         <v>34</v>
@@ -5544,22 +5562,22 @@
         <v>63</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="F49" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G49" s="15" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="I49" s="15" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="J49" s="16" t="s">
         <v>34</v>
@@ -5598,22 +5616,22 @@
         <v>63</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="F50" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G50" s="15" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="I50" s="15" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="J50" s="16" t="s">
         <v>34</v>
@@ -5652,22 +5670,22 @@
         <v>63</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="F51" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="H51" s="15" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="I51" s="15" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="J51" s="16" t="s">
         <v>34</v>
@@ -5706,22 +5724,22 @@
         <v>63</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="F52" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G52" s="15" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="H52" s="15" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="I52" s="15" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="J52" s="16" t="s">
         <v>34</v>
@@ -5760,22 +5778,22 @@
         <v>63</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="E53" s="13" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="F53" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G53" s="15" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="H53" s="15" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="I53" s="15" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="J53" s="16" t="s">
         <v>34</v>
@@ -5814,22 +5832,22 @@
         <v>63</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="E54" s="13" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="F54" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G54" s="15" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="H54" s="15" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="I54" s="15" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="J54" s="16" t="s">
         <v>34</v>
@@ -5868,22 +5886,22 @@
         <v>63</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="E55" s="13" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="F55" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G55" s="15" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="H55" s="15" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="I55" s="15" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="J55" s="16" t="s">
         <v>34</v>
@@ -5922,22 +5940,22 @@
         <v>63</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="E56" s="13" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="F56" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G56" s="15" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="H56" s="15" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="I56" s="15" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="J56" s="16" t="s">
         <v>34</v>
@@ -5976,22 +5994,22 @@
         <v>63</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="E57" s="13" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="F57" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G57" s="15" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="H57" s="15" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="I57" s="15" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="J57" s="16" t="s">
         <v>34</v>
@@ -6030,22 +6048,22 @@
         <v>59</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="F58" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G58" s="15" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="H58" s="15" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="I58" s="15" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="J58" s="16" t="s">
         <v>34</v>
@@ -6074,22 +6092,22 @@
         <v>59</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="F59" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G59" s="15" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="H59" s="15" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="I59" s="15" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="J59" s="16" t="s">
         <v>34</v>
@@ -6118,22 +6136,22 @@
         <v>59</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="F60" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G60" s="15" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="H60" s="15" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="I60" s="15" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="J60" s="16" t="s">
         <v>34</v>
@@ -6162,22 +6180,22 @@
         <v>59</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="E61" s="13" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="F61" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G61" s="15" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="H61" s="15" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="I61" s="15" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="J61" s="16" t="s">
         <v>34</v>
@@ -6206,22 +6224,22 @@
         <v>59</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="E62" s="13" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="F62" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G62" s="15" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="H62" s="15" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="I62" s="15" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="J62" s="16" t="s">
         <v>34</v>
@@ -6260,22 +6278,22 @@
         <v>59</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="E63" s="13" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="F63" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G63" s="15" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="H63" s="15" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="I63" s="15" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="J63" s="16" t="s">
         <v>34</v>
@@ -6314,22 +6332,22 @@
         <v>59</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="E64" s="13" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="F64" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G64" s="15" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="H64" s="15" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="I64" s="15" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="J64" s="16" t="s">
         <v>34</v>
@@ -6368,22 +6386,22 @@
         <v>59</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="E65" s="13" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="F65" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G65" s="15" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="H65" s="15" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="I65" s="15" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="J65" s="16" t="s">
         <v>34</v>
@@ -6422,22 +6440,22 @@
         <v>59</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="E66" s="13" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="F66" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G66" s="15" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="H66" s="15" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="I66" s="15" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="J66" s="16" t="s">
         <v>34</v>
@@ -6476,22 +6494,22 @@
         <v>59</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="E67" s="13" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="F67" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G67" s="15" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="H67" s="15" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="I67" s="15" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="J67" s="16" t="s">
         <v>34</v>
@@ -6530,22 +6548,22 @@
         <v>59</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="E68" s="13" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="F68" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G68" s="15" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="H68" s="15" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="I68" s="15" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="J68" s="16" t="s">
         <v>34</v>
@@ -6584,22 +6602,22 @@
         <v>59</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="E69" s="13" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="F69" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G69" s="15" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="H69" s="15" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="I69" s="15" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="J69" s="16" t="s">
         <v>34</v>
@@ -6638,22 +6656,22 @@
         <v>59</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="E70" s="13" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="F70" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G70" s="15" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="H70" s="15" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="I70" s="15" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="J70" s="16" t="s">
         <v>34</v>
@@ -6692,22 +6710,22 @@
         <v>59</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="E71" s="13" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="F71" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G71" s="15" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="H71" s="15" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="I71" s="15" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="J71" s="16" t="s">
         <v>34</v>
@@ -6746,22 +6764,22 @@
         <v>59</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="E72" s="13" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="F72" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G72" s="15" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="H72" s="15" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="I72" s="15" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="J72" s="16" t="s">
         <v>34</v>
@@ -6800,22 +6818,22 @@
         <v>59</v>
       </c>
       <c r="D73" s="12" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="E73" s="13" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="F73" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G73" s="15" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="H73" s="15" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="I73" s="15" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="J73" s="16" t="s">
         <v>34</v>
@@ -6854,22 +6872,22 @@
         <v>59</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="E74" s="13" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="F74" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G74" s="15" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="H74" s="15" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="I74" s="15" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="J74" s="16" t="s">
         <v>34</v>
@@ -6908,22 +6926,22 @@
         <v>59</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="E75" s="13" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="F75" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G75" s="15" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="H75" s="15" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="I75" s="15" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="J75" s="16" t="s">
         <v>34</v>
@@ -6962,22 +6980,22 @@
         <v>59</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="E76" s="13" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="F76" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G76" s="15" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="H76" s="15" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="I76" s="15" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="J76" s="16" t="s">
         <v>34</v>
@@ -7016,22 +7034,22 @@
         <v>59</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="E77" s="13" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="F77" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G77" s="15" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="H77" s="15" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="I77" s="15" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="J77" s="16" t="s">
         <v>34</v>
@@ -7070,22 +7088,22 @@
         <v>59</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="E78" s="13" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="F78" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G78" s="15" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="H78" s="15" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="I78" s="15" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="J78" s="16" t="s">
         <v>34</v>
@@ -7118,28 +7136,28 @@
         <v>208</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C79" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="E79" s="13" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="F79" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G79" s="15" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="H79" s="15" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="I79" s="15" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="J79" s="16" t="s">
         <v>34</v>
@@ -7162,28 +7180,28 @@
         <v>209</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="C80" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D80" s="12" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="E80" s="13" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="F80" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G80" s="15" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="H80" s="15" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="I80" s="15" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="J80" s="16" t="s">
         <v>34</v>
@@ -7206,28 +7224,28 @@
         <v>210</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C81" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D81" s="12" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="E81" s="13" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="F81" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G81" s="15" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="H81" s="15" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="I81" s="15" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="J81" s="16" t="s">
         <v>34</v>
@@ -7250,28 +7268,28 @@
         <v>211</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="C82" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="E82" s="13" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="F82" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G82" s="15" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="H82" s="15" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="I82" s="15" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="J82" s="16" t="s">
         <v>34</v>
@@ -7294,28 +7312,28 @@
         <v>212</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="C83" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D83" s="12" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="E83" s="13" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="F83" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G83" s="15" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="H83" s="15" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="I83" s="15" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="J83" s="16" t="s">
         <v>34</v>
@@ -7338,25 +7356,25 @@
         <v>213</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C84" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D84" s="12" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="E84" s="13" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="F84" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G84" s="15" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="H84" s="15" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="I84" s="15"/>
       <c r="J84" s="16" t="s">
@@ -7390,25 +7408,25 @@
         <v>214</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C85" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D85" s="12" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="E85" s="13" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="F85" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G85" s="15" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="H85" s="15" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="I85" s="15"/>
       <c r="J85" s="16" t="s">
@@ -7442,28 +7460,28 @@
         <v>215</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C86" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D86" s="12" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="E86" s="13" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="F86" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G86" s="15" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="H86" s="15" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="I86" s="15" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="J86" s="16" t="s">
         <v>34</v>
@@ -7486,25 +7504,25 @@
         <v>216</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C87" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D87" s="12" t="s">
-        <v>402</v>
+        <v>408</v>
       </c>
       <c r="E87" s="13" t="s">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="F87" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G87" s="15" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
       <c r="H87" s="15" t="s">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="I87" s="15"/>
       <c r="J87" s="16" t="s">
@@ -7528,28 +7546,28 @@
         <v>217</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C88" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D88" s="12" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="E88" s="13" t="s">
-        <v>407</v>
+        <v>413</v>
       </c>
       <c r="F88" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G88" s="15" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="H88" s="15" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="I88" s="15" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="J88" s="16" t="s">
         <v>34</v>
@@ -7572,28 +7590,28 @@
         <v>218</v>
       </c>
       <c r="B89" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C89" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D89" s="12" t="s">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c r="E89" s="13" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="F89" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G89" s="15" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="H89" s="15" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="I89" s="15" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="J89" s="16" t="s">
         <v>34</v>
@@ -7616,28 +7634,28 @@
         <v>219</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C90" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D90" s="12" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="E90" s="13" t="s">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="F90" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G90" s="15" t="s">
-        <v>418</v>
+        <v>424</v>
       </c>
       <c r="H90" s="15" t="s">
-        <v>419</v>
+        <v>425</v>
       </c>
       <c r="I90" s="15" t="s">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="J90" s="16" t="s">
         <v>34</v>
@@ -7660,25 +7678,25 @@
         <v>220</v>
       </c>
       <c r="B91" s="12" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="C91" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D91" s="12" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="E91" s="13" t="s">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="F91" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G91" s="15" t="s">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="H91" s="15" t="s">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="I91" s="15"/>
       <c r="J91" s="16" t="s">
@@ -7692,13 +7710,13 @@
         <v>34</v>
       </c>
       <c r="N91" s="16" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="O91" s="16" t="s">
         <v>34</v>
       </c>
       <c r="P91" s="16" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="Q91" s="16"/>
       <c r="R91" s="17"/>
@@ -7712,25 +7730,25 @@
         <v>221</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C92" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D92" s="12" t="s">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="E92" s="13" t="s">
-        <v>428</v>
+        <v>434</v>
       </c>
       <c r="F92" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G92" s="15" t="s">
-        <v>429</v>
+        <v>435</v>
       </c>
       <c r="H92" s="15" t="s">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c r="I92" s="15"/>
       <c r="J92" s="16" t="s">
@@ -7744,13 +7762,13 @@
         <v>34</v>
       </c>
       <c r="N92" s="16" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="O92" s="16" t="s">
         <v>34</v>
       </c>
       <c r="P92" s="16" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="Q92" s="16"/>
       <c r="R92" s="17"/>
@@ -7764,25 +7782,25 @@
         <v>222</v>
       </c>
       <c r="B93" s="12" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="C93" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D93" s="12" t="s">
-        <v>431</v>
+        <v>437</v>
       </c>
       <c r="E93" s="13" t="s">
-        <v>432</v>
+        <v>438</v>
       </c>
       <c r="F93" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G93" s="15" t="s">
-        <v>433</v>
+        <v>439</v>
       </c>
       <c r="H93" s="15" t="s">
-        <v>434</v>
+        <v>440</v>
       </c>
       <c r="I93" s="15"/>
       <c r="J93" s="16" t="s">
@@ -7796,13 +7814,13 @@
         <v>34</v>
       </c>
       <c r="N93" s="16" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="O93" s="16" t="s">
         <v>34</v>
       </c>
       <c r="P93" s="16" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="Q93" s="16"/>
       <c r="R93" s="17"/>
@@ -7816,25 +7834,25 @@
         <v>223</v>
       </c>
       <c r="B94" s="12" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="C94" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D94" s="12" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="E94" s="13" t="s">
-        <v>436</v>
+        <v>442</v>
       </c>
       <c r="F94" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G94" s="15" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="H94" s="15" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="I94" s="15"/>
       <c r="J94" s="16" t="s">
@@ -7848,13 +7866,13 @@
         <v>34</v>
       </c>
       <c r="N94" s="16" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="O94" s="16" t="s">
         <v>34</v>
       </c>
       <c r="P94" s="16" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="Q94" s="16"/>
       <c r="R94" s="17"/>
@@ -7868,28 +7886,28 @@
         <v>288</v>
       </c>
       <c r="B95" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C95" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D95" s="12" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
       <c r="E95" s="13" t="s">
-        <v>440</v>
+        <v>446</v>
       </c>
       <c r="F95" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G95" s="15" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="H95" s="15" t="s">
-        <v>442</v>
+        <v>448</v>
       </c>
       <c r="I95" s="15" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="J95" s="16" t="s">
         <v>34</v>
@@ -7912,28 +7930,28 @@
         <v>289</v>
       </c>
       <c r="B96" s="12" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="C96" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D96" s="12" t="s">
-        <v>444</v>
+        <v>450</v>
       </c>
       <c r="E96" s="13" t="s">
-        <v>445</v>
+        <v>451</v>
       </c>
       <c r="F96" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G96" s="15" t="s">
-        <v>446</v>
+        <v>452</v>
       </c>
       <c r="H96" s="15" t="s">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="I96" s="15" t="s">
-        <v>448</v>
+        <v>454</v>
       </c>
       <c r="J96" s="16" t="s">
         <v>34</v>
@@ -7956,28 +7974,28 @@
         <v>290</v>
       </c>
       <c r="B97" s="12" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C97" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D97" s="12" t="s">
-        <v>449</v>
+        <v>455</v>
       </c>
       <c r="E97" s="13" t="s">
-        <v>450</v>
+        <v>456</v>
       </c>
       <c r="F97" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G97" s="15" t="s">
-        <v>451</v>
+        <v>457</v>
       </c>
       <c r="H97" s="15" t="s">
-        <v>452</v>
+        <v>458</v>
       </c>
       <c r="I97" s="15" t="s">
-        <v>453</v>
+        <v>459</v>
       </c>
       <c r="J97" s="16" t="s">
         <v>34</v>
@@ -8000,28 +8018,28 @@
         <v>291</v>
       </c>
       <c r="B98" s="12" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="C98" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D98" s="12" t="s">
-        <v>454</v>
+        <v>460</v>
       </c>
       <c r="E98" s="13" t="s">
-        <v>455</v>
+        <v>461</v>
       </c>
       <c r="F98" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G98" s="15" t="s">
-        <v>456</v>
+        <v>462</v>
       </c>
       <c r="H98" s="15" t="s">
-        <v>457</v>
+        <v>463</v>
       </c>
       <c r="I98" s="15" t="s">
-        <v>458</v>
+        <v>464</v>
       </c>
       <c r="J98" s="16" t="s">
         <v>34</v>
@@ -8044,28 +8062,28 @@
         <v>292</v>
       </c>
       <c r="B99" s="12" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="C99" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>459</v>
+        <v>465</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>460</v>
+        <v>466</v>
       </c>
       <c r="F99" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G99" s="15" t="s">
-        <v>461</v>
+        <v>467</v>
       </c>
       <c r="H99" s="15" t="s">
-        <v>462</v>
+        <v>468</v>
       </c>
       <c r="I99" s="15" t="s">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="J99" s="16" t="s">
         <v>34</v>
@@ -8088,25 +8106,25 @@
         <v>293</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C100" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D100" s="12" t="s">
-        <v>464</v>
+        <v>470</v>
       </c>
       <c r="E100" s="13" t="s">
-        <v>465</v>
+        <v>471</v>
       </c>
       <c r="F100" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G100" s="15" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="H100" s="15" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="I100" s="15"/>
       <c r="J100" s="16" t="s">
@@ -8140,25 +8158,25 @@
         <v>294</v>
       </c>
       <c r="B101" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C101" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D101" s="12" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="F101" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G101" s="15" t="s">
-        <v>470</v>
+        <v>476</v>
       </c>
       <c r="H101" s="15" t="s">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="I101" s="15"/>
       <c r="J101" s="16" t="s">
@@ -8192,28 +8210,28 @@
         <v>295</v>
       </c>
       <c r="B102" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C102" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D102" s="12" t="s">
-        <v>472</v>
+        <v>478</v>
       </c>
       <c r="E102" s="13" t="s">
-        <v>473</v>
+        <v>479</v>
       </c>
       <c r="F102" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G102" s="15" t="s">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="H102" s="15" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="I102" s="15" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="J102" s="16" t="s">
         <v>34</v>
@@ -8236,25 +8254,25 @@
         <v>296</v>
       </c>
       <c r="B103" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C103" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D103" s="12" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="E103" s="13" t="s">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="F103" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G103" s="15" t="s">
-        <v>479</v>
+        <v>485</v>
       </c>
       <c r="H103" s="15" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="I103" s="15"/>
       <c r="J103" s="16" t="s">
@@ -8278,28 +8296,28 @@
         <v>297</v>
       </c>
       <c r="B104" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C104" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D104" s="12" t="s">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="E104" s="13" t="s">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="F104" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G104" s="15" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="H104" s="15" t="s">
-        <v>484</v>
+        <v>490</v>
       </c>
       <c r="I104" s="15" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="J104" s="16" t="s">
         <v>34</v>
@@ -8322,28 +8340,28 @@
         <v>298</v>
       </c>
       <c r="B105" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C105" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D105" s="12" t="s">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="E105" s="13" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="F105" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G105" s="15" t="s">
-        <v>488</v>
+        <v>494</v>
       </c>
       <c r="H105" s="15" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
       <c r="I105" s="15" t="s">
-        <v>490</v>
+        <v>496</v>
       </c>
       <c r="J105" s="16" t="s">
         <v>34</v>
@@ -8366,28 +8384,28 @@
         <v>299</v>
       </c>
       <c r="B106" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C106" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D106" s="12" t="s">
-        <v>491</v>
+        <v>497</v>
       </c>
       <c r="E106" s="13" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="F106" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G106" s="15" t="s">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="H106" s="15" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="I106" s="15" t="s">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="J106" s="16" t="s">
         <v>34</v>
@@ -8410,25 +8428,25 @@
         <v>300</v>
       </c>
       <c r="B107" s="12" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="C107" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D107" s="12" t="s">
-        <v>496</v>
+        <v>502</v>
       </c>
       <c r="E107" s="13" t="s">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="F107" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G107" s="15" t="s">
-        <v>497</v>
+        <v>503</v>
       </c>
       <c r="H107" s="15" t="s">
-        <v>498</v>
+        <v>504</v>
       </c>
       <c r="I107" s="15"/>
       <c r="J107" s="16" t="s">
@@ -8442,13 +8460,13 @@
         <v>34</v>
       </c>
       <c r="N107" s="16" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="O107" s="16" t="s">
         <v>34</v>
       </c>
       <c r="P107" s="16" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="Q107" s="16"/>
       <c r="R107" s="17"/>
@@ -8462,25 +8480,25 @@
         <v>301</v>
       </c>
       <c r="B108" s="12" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C108" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D108" s="12" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="E108" s="13" t="s">
-        <v>500</v>
+        <v>506</v>
       </c>
       <c r="F108" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G108" s="15" t="s">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="H108" s="15" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="I108" s="15"/>
       <c r="J108" s="16" t="s">
@@ -8494,13 +8512,13 @@
         <v>34</v>
       </c>
       <c r="N108" s="16" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="O108" s="16" t="s">
         <v>34</v>
       </c>
       <c r="P108" s="16" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="Q108" s="16"/>
       <c r="R108" s="17"/>
@@ -8514,25 +8532,25 @@
         <v>302</v>
       </c>
       <c r="B109" s="12" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="C109" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D109" s="12" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="E109" s="13" t="s">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="F109" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G109" s="15" t="s">
-        <v>505</v>
+        <v>511</v>
       </c>
       <c r="H109" s="15" t="s">
-        <v>506</v>
+        <v>512</v>
       </c>
       <c r="I109" s="15"/>
       <c r="J109" s="16" t="s">
@@ -8546,13 +8564,13 @@
         <v>34</v>
       </c>
       <c r="N109" s="16" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="O109" s="16" t="s">
         <v>34</v>
       </c>
       <c r="P109" s="16" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="Q109" s="16"/>
       <c r="R109" s="17"/>
@@ -8566,25 +8584,25 @@
         <v>303</v>
       </c>
       <c r="B110" s="12" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="C110" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D110" s="12" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
       <c r="E110" s="13" t="s">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="F110" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G110" s="15" t="s">
-        <v>509</v>
+        <v>515</v>
       </c>
       <c r="H110" s="15" t="s">
-        <v>510</v>
+        <v>516</v>
       </c>
       <c r="I110" s="15"/>
       <c r="J110" s="16" t="s">
@@ -8598,13 +8616,13 @@
         <v>34</v>
       </c>
       <c r="N110" s="16" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="O110" s="16" t="s">
         <v>34</v>
       </c>
       <c r="P110" s="16" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="Q110" s="16"/>
       <c r="R110" s="17"/>
@@ -8618,28 +8636,28 @@
         <v>304</v>
       </c>
       <c r="B111" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C111" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D111" s="12" t="s">
-        <v>511</v>
+        <v>517</v>
       </c>
       <c r="E111" s="13" t="s">
-        <v>512</v>
+        <v>518</v>
       </c>
       <c r="F111" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G111" s="15" t="s">
-        <v>513</v>
+        <v>519</v>
       </c>
       <c r="H111" s="15" t="s">
-        <v>514</v>
+        <v>520</v>
       </c>
       <c r="I111" s="15" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="J111" s="16" t="s">
         <v>34</v>
@@ -8662,28 +8680,28 @@
         <v>305</v>
       </c>
       <c r="B112" s="12" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="C112" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D112" s="12" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="E112" s="13" t="s">
-        <v>517</v>
+        <v>523</v>
       </c>
       <c r="F112" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G112" s="15" t="s">
-        <v>518</v>
+        <v>524</v>
       </c>
       <c r="H112" s="15" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="I112" s="15" t="s">
-        <v>520</v>
+        <v>526</v>
       </c>
       <c r="J112" s="16" t="s">
         <v>34</v>
@@ -8706,28 +8724,28 @@
         <v>306</v>
       </c>
       <c r="B113" s="12" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C113" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D113" s="12" t="s">
-        <v>521</v>
+        <v>527</v>
       </c>
       <c r="E113" s="13" t="s">
-        <v>522</v>
+        <v>528</v>
       </c>
       <c r="F113" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G113" s="15" t="s">
-        <v>523</v>
+        <v>529</v>
       </c>
       <c r="H113" s="15" t="s">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="I113" s="15" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="J113" s="16" t="s">
         <v>34</v>
@@ -8750,28 +8768,28 @@
         <v>307</v>
       </c>
       <c r="B114" s="12" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="C114" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D114" s="12" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="E114" s="13" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="F114" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G114" s="15" t="s">
-        <v>528</v>
+        <v>534</v>
       </c>
       <c r="H114" s="15" t="s">
-        <v>529</v>
+        <v>535</v>
       </c>
       <c r="I114" s="15" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="J114" s="16" t="s">
         <v>34</v>
@@ -8794,28 +8812,28 @@
         <v>308</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="C115" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D115" s="12" t="s">
-        <v>531</v>
+        <v>537</v>
       </c>
       <c r="E115" s="13" t="s">
-        <v>532</v>
+        <v>538</v>
       </c>
       <c r="F115" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G115" s="15" t="s">
-        <v>533</v>
+        <v>539</v>
       </c>
       <c r="H115" s="15" t="s">
-        <v>534</v>
+        <v>540</v>
       </c>
       <c r="I115" s="15" t="s">
-        <v>535</v>
+        <v>541</v>
       </c>
       <c r="J115" s="16" t="s">
         <v>34</v>
@@ -8838,25 +8856,25 @@
         <v>309</v>
       </c>
       <c r="B116" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C116" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D116" s="12" t="s">
-        <v>536</v>
+        <v>542</v>
       </c>
       <c r="E116" s="13" t="s">
-        <v>537</v>
+        <v>543</v>
       </c>
       <c r="F116" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G116" s="15" t="s">
-        <v>538</v>
+        <v>544</v>
       </c>
       <c r="H116" s="15" t="s">
-        <v>539</v>
+        <v>545</v>
       </c>
       <c r="I116" s="15"/>
       <c r="J116" s="16" t="s">
@@ -8890,25 +8908,25 @@
         <v>310</v>
       </c>
       <c r="B117" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C117" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D117" s="12" t="s">
-        <v>540</v>
+        <v>546</v>
       </c>
       <c r="E117" s="13" t="s">
-        <v>541</v>
+        <v>547</v>
       </c>
       <c r="F117" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G117" s="15" t="s">
-        <v>542</v>
+        <v>548</v>
       </c>
       <c r="H117" s="15" t="s">
-        <v>543</v>
+        <v>549</v>
       </c>
       <c r="I117" s="15"/>
       <c r="J117" s="16" t="s">
@@ -8942,28 +8960,28 @@
         <v>311</v>
       </c>
       <c r="B118" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C118" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D118" s="12" t="s">
-        <v>544</v>
+        <v>550</v>
       </c>
       <c r="E118" s="13" t="s">
-        <v>545</v>
+        <v>551</v>
       </c>
       <c r="F118" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G118" s="15" t="s">
-        <v>546</v>
+        <v>552</v>
       </c>
       <c r="H118" s="15" t="s">
-        <v>547</v>
+        <v>553</v>
       </c>
       <c r="I118" s="15" t="s">
-        <v>548</v>
+        <v>554</v>
       </c>
       <c r="J118" s="16" t="s">
         <v>34</v>
@@ -8986,25 +9004,25 @@
         <v>312</v>
       </c>
       <c r="B119" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C119" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D119" s="12" t="s">
-        <v>549</v>
+        <v>555</v>
       </c>
       <c r="E119" s="13" t="s">
-        <v>550</v>
+        <v>556</v>
       </c>
       <c r="F119" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G119" s="15" t="s">
-        <v>551</v>
+        <v>557</v>
       </c>
       <c r="H119" s="15" t="s">
-        <v>552</v>
+        <v>558</v>
       </c>
       <c r="I119" s="15"/>
       <c r="J119" s="16" t="s">
@@ -9028,28 +9046,28 @@
         <v>313</v>
       </c>
       <c r="B120" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C120" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D120" s="12" t="s">
-        <v>553</v>
+        <v>559</v>
       </c>
       <c r="E120" s="13" t="s">
-        <v>554</v>
+        <v>560</v>
       </c>
       <c r="F120" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G120" s="15" t="s">
-        <v>555</v>
+        <v>561</v>
       </c>
       <c r="H120" s="15" t="s">
-        <v>556</v>
+        <v>562</v>
       </c>
       <c r="I120" s="15" t="s">
-        <v>557</v>
+        <v>563</v>
       </c>
       <c r="J120" s="16" t="s">
         <v>34</v>
@@ -9072,28 +9090,28 @@
         <v>314</v>
       </c>
       <c r="B121" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C121" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D121" s="12" t="s">
-        <v>558</v>
+        <v>564</v>
       </c>
       <c r="E121" s="13" t="s">
-        <v>559</v>
+        <v>565</v>
       </c>
       <c r="F121" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G121" s="15" t="s">
-        <v>560</v>
+        <v>566</v>
       </c>
       <c r="H121" s="15" t="s">
-        <v>561</v>
+        <v>567</v>
       </c>
       <c r="I121" s="15" t="s">
-        <v>562</v>
+        <v>568</v>
       </c>
       <c r="J121" s="16" t="s">
         <v>34</v>
@@ -9116,28 +9134,28 @@
         <v>315</v>
       </c>
       <c r="B122" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C122" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D122" s="12" t="s">
-        <v>563</v>
+        <v>569</v>
       </c>
       <c r="E122" s="13" t="s">
-        <v>564</v>
+        <v>570</v>
       </c>
       <c r="F122" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G122" s="15" t="s">
-        <v>565</v>
+        <v>571</v>
       </c>
       <c r="H122" s="15" t="s">
-        <v>566</v>
+        <v>572</v>
       </c>
       <c r="I122" s="15" t="s">
-        <v>567</v>
+        <v>573</v>
       </c>
       <c r="J122" s="16" t="s">
         <v>34</v>
@@ -9160,25 +9178,25 @@
         <v>316</v>
       </c>
       <c r="B123" s="12" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="C123" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D123" s="12" t="s">
-        <v>568</v>
+        <v>574</v>
       </c>
       <c r="E123" s="13" t="s">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="F123" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G123" s="15" t="s">
-        <v>569</v>
+        <v>575</v>
       </c>
       <c r="H123" s="15" t="s">
-        <v>570</v>
+        <v>576</v>
       </c>
       <c r="I123" s="15"/>
       <c r="J123" s="16" t="s">
@@ -9192,13 +9210,13 @@
         <v>34</v>
       </c>
       <c r="N123" s="16" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="O123" s="16" t="s">
         <v>34</v>
       </c>
       <c r="P123" s="16" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="Q123" s="16"/>
       <c r="R123" s="17"/>
@@ -9212,25 +9230,25 @@
         <v>317</v>
       </c>
       <c r="B124" s="12" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C124" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D124" s="12" t="s">
-        <v>571</v>
+        <v>577</v>
       </c>
       <c r="E124" s="13" t="s">
-        <v>572</v>
+        <v>578</v>
       </c>
       <c r="F124" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G124" s="15" t="s">
-        <v>573</v>
+        <v>579</v>
       </c>
       <c r="H124" s="15" t="s">
-        <v>574</v>
+        <v>580</v>
       </c>
       <c r="I124" s="15"/>
       <c r="J124" s="16" t="s">
@@ -9244,13 +9262,13 @@
         <v>34</v>
       </c>
       <c r="N124" s="16" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="O124" s="16" t="s">
         <v>34</v>
       </c>
       <c r="P124" s="16" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="Q124" s="16"/>
       <c r="R124" s="17"/>
@@ -9264,25 +9282,25 @@
         <v>318</v>
       </c>
       <c r="B125" s="12" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="C125" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D125" s="12" t="s">
-        <v>575</v>
+        <v>581</v>
       </c>
       <c r="E125" s="13" t="s">
-        <v>576</v>
+        <v>582</v>
       </c>
       <c r="F125" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G125" s="15" t="s">
-        <v>577</v>
+        <v>583</v>
       </c>
       <c r="H125" s="15" t="s">
-        <v>578</v>
+        <v>584</v>
       </c>
       <c r="I125" s="15"/>
       <c r="J125" s="16" t="s">
@@ -9296,13 +9314,13 @@
         <v>34</v>
       </c>
       <c r="N125" s="16" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="O125" s="16" t="s">
         <v>34</v>
       </c>
       <c r="P125" s="16" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="Q125" s="16"/>
       <c r="R125" s="17"/>
@@ -9316,25 +9334,25 @@
         <v>319</v>
       </c>
       <c r="B126" s="12" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="C126" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D126" s="12" t="s">
-        <v>579</v>
+        <v>585</v>
       </c>
       <c r="E126" s="13" t="s">
-        <v>580</v>
+        <v>586</v>
       </c>
       <c r="F126" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G126" s="15" t="s">
-        <v>581</v>
+        <v>587</v>
       </c>
       <c r="H126" s="15" t="s">
-        <v>582</v>
+        <v>588</v>
       </c>
       <c r="I126" s="15"/>
       <c r="J126" s="16" t="s">
@@ -9348,13 +9366,13 @@
         <v>34</v>
       </c>
       <c r="N126" s="16" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="O126" s="16" t="s">
         <v>34</v>
       </c>
       <c r="P126" s="16" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="Q126" s="16"/>
       <c r="R126" s="17"/>
@@ -9368,25 +9386,25 @@
         <v>324</v>
       </c>
       <c r="B127" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C127" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D127" s="12" t="s">
-        <v>583</v>
+        <v>589</v>
       </c>
       <c r="E127" s="13" t="s">
-        <v>584</v>
+        <v>590</v>
       </c>
       <c r="F127" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G127" s="15" t="s">
-        <v>585</v>
+        <v>591</v>
       </c>
       <c r="H127" s="15" t="s">
-        <v>586</v>
+        <v>592</v>
       </c>
       <c r="I127" s="15"/>
       <c r="J127" s="16" t="s">
@@ -9420,25 +9438,25 @@
         <v>325</v>
       </c>
       <c r="B128" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C128" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D128" s="12" t="s">
-        <v>587</v>
+        <v>593</v>
       </c>
       <c r="E128" s="13" t="s">
-        <v>588</v>
+        <v>594</v>
       </c>
       <c r="F128" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G128" s="15" t="s">
-        <v>589</v>
+        <v>595</v>
       </c>
       <c r="H128" s="15" t="s">
-        <v>590</v>
+        <v>596</v>
       </c>
       <c r="I128" s="15"/>
       <c r="J128" s="16" t="s">
@@ -9472,25 +9490,25 @@
         <v>326</v>
       </c>
       <c r="B129" s="12" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="C129" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D129" s="12" t="s">
-        <v>591</v>
+        <v>597</v>
       </c>
       <c r="E129" s="13" t="s">
-        <v>592</v>
+        <v>598</v>
       </c>
       <c r="F129" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G129" s="15" t="s">
-        <v>593</v>
+        <v>599</v>
       </c>
       <c r="H129" s="15" t="s">
-        <v>594</v>
+        <v>600</v>
       </c>
       <c r="I129" s="15"/>
       <c r="J129" s="16" t="s">
@@ -9524,25 +9542,25 @@
         <v>327</v>
       </c>
       <c r="B130" s="12" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="C130" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D130" s="12" t="s">
-        <v>595</v>
+        <v>601</v>
       </c>
       <c r="E130" s="13" t="s">
-        <v>596</v>
+        <v>602</v>
       </c>
       <c r="F130" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G130" s="15" t="s">
-        <v>597</v>
+        <v>603</v>
       </c>
       <c r="H130" s="15" t="s">
-        <v>598</v>
+        <v>604</v>
       </c>
       <c r="I130" s="15"/>
       <c r="J130" s="16" t="s">
@@ -9576,25 +9594,25 @@
         <v>344</v>
       </c>
       <c r="B131" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C131" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D131" s="12" t="s">
-        <v>599</v>
+        <v>605</v>
       </c>
       <c r="E131" s="13" t="s">
-        <v>600</v>
+        <v>606</v>
       </c>
       <c r="F131" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G131" s="15" t="s">
-        <v>601</v>
+        <v>607</v>
       </c>
       <c r="H131" s="15" t="s">
-        <v>602</v>
+        <v>608</v>
       </c>
       <c r="I131" s="15"/>
       <c r="J131" s="16" t="s">
@@ -9628,25 +9646,25 @@
         <v>345</v>
       </c>
       <c r="B132" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C132" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D132" s="12" t="s">
-        <v>603</v>
+        <v>609</v>
       </c>
       <c r="E132" s="13" t="s">
-        <v>604</v>
+        <v>610</v>
       </c>
       <c r="F132" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G132" s="15" t="s">
-        <v>605</v>
+        <v>611</v>
       </c>
       <c r="H132" s="15" t="s">
-        <v>606</v>
+        <v>612</v>
       </c>
       <c r="I132" s="15"/>
       <c r="J132" s="16" t="s">
@@ -9680,25 +9698,25 @@
         <v>346</v>
       </c>
       <c r="B133" s="12" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="C133" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D133" s="12" t="s">
-        <v>607</v>
+        <v>613</v>
       </c>
       <c r="E133" s="13" t="s">
-        <v>608</v>
+        <v>614</v>
       </c>
       <c r="F133" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G133" s="15" t="s">
-        <v>609</v>
+        <v>615</v>
       </c>
       <c r="H133" s="15" t="s">
-        <v>610</v>
+        <v>616</v>
       </c>
       <c r="I133" s="15"/>
       <c r="J133" s="16" t="s">
@@ -9732,25 +9750,25 @@
         <v>347</v>
       </c>
       <c r="B134" s="12" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="C134" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D134" s="12" t="s">
-        <v>611</v>
+        <v>617</v>
       </c>
       <c r="E134" s="13" t="s">
-        <v>612</v>
+        <v>618</v>
       </c>
       <c r="F134" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G134" s="15" t="s">
-        <v>613</v>
+        <v>619</v>
       </c>
       <c r="H134" s="15" t="s">
-        <v>614</v>
+        <v>620</v>
       </c>
       <c r="I134" s="15"/>
       <c r="J134" s="16" t="s">
@@ -9784,25 +9802,25 @@
         <v>348</v>
       </c>
       <c r="B135" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C135" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D135" s="12" t="s">
-        <v>615</v>
+        <v>621</v>
       </c>
       <c r="E135" s="13" t="s">
-        <v>616</v>
+        <v>622</v>
       </c>
       <c r="F135" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G135" s="15" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="H135" s="15" t="s">
-        <v>618</v>
+        <v>624</v>
       </c>
       <c r="I135" s="15"/>
       <c r="J135" s="16" t="s">
@@ -9836,25 +9854,25 @@
         <v>349</v>
       </c>
       <c r="B136" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C136" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D136" s="12" t="s">
-        <v>619</v>
+        <v>625</v>
       </c>
       <c r="E136" s="13" t="s">
-        <v>620</v>
+        <v>626</v>
       </c>
       <c r="F136" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G136" s="15" t="s">
-        <v>621</v>
+        <v>627</v>
       </c>
       <c r="H136" s="15" t="s">
-        <v>622</v>
+        <v>628</v>
       </c>
       <c r="I136" s="15"/>
       <c r="J136" s="16" t="s">
@@ -9888,25 +9906,25 @@
         <v>350</v>
       </c>
       <c r="B137" s="12" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="C137" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D137" s="12" t="s">
-        <v>623</v>
+        <v>629</v>
       </c>
       <c r="E137" s="13" t="s">
-        <v>624</v>
+        <v>630</v>
       </c>
       <c r="F137" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G137" s="15" t="s">
-        <v>625</v>
+        <v>631</v>
       </c>
       <c r="H137" s="15" t="s">
-        <v>626</v>
+        <v>632</v>
       </c>
       <c r="I137" s="15"/>
       <c r="J137" s="16" t="s">
@@ -9940,25 +9958,25 @@
         <v>351</v>
       </c>
       <c r="B138" s="12" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="C138" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D138" s="12" t="s">
-        <v>627</v>
+        <v>633</v>
       </c>
       <c r="E138" s="13" t="s">
-        <v>628</v>
+        <v>634</v>
       </c>
       <c r="F138" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G138" s="15" t="s">
-        <v>629</v>
+        <v>635</v>
       </c>
       <c r="H138" s="15" t="s">
-        <v>630</v>
+        <v>636</v>
       </c>
       <c r="I138" s="15"/>
       <c r="J138" s="16" t="s">
@@ -9992,25 +10010,25 @@
         <v>354</v>
       </c>
       <c r="B139" s="12" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C139" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D139" s="12" t="s">
-        <v>631</v>
+        <v>637</v>
       </c>
       <c r="E139" s="13" t="s">
-        <v>632</v>
+        <v>638</v>
       </c>
       <c r="F139" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G139" s="15" t="s">
-        <v>633</v>
+        <v>639</v>
       </c>
       <c r="H139" s="15" t="s">
-        <v>634</v>
+        <v>640</v>
       </c>
       <c r="I139" s="15"/>
       <c r="J139" s="16" t="s">
@@ -10044,25 +10062,25 @@
         <v>355</v>
       </c>
       <c r="B140" s="12" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C140" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D140" s="12" t="s">
-        <v>635</v>
+        <v>641</v>
       </c>
       <c r="E140" s="13" t="s">
-        <v>636</v>
+        <v>642</v>
       </c>
       <c r="F140" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G140" s="15" t="s">
-        <v>637</v>
+        <v>643</v>
       </c>
       <c r="H140" s="15" t="s">
-        <v>638</v>
+        <v>644</v>
       </c>
       <c r="I140" s="15"/>
       <c r="J140" s="16" t="s">
@@ -10096,25 +10114,25 @@
         <v>364</v>
       </c>
       <c r="B141" s="12" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C141" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D141" s="12" t="s">
-        <v>639</v>
+        <v>645</v>
       </c>
       <c r="E141" s="13" t="s">
-        <v>640</v>
+        <v>646</v>
       </c>
       <c r="F141" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G141" s="15" t="s">
-        <v>641</v>
+        <v>647</v>
       </c>
       <c r="H141" s="15" t="s">
-        <v>642</v>
+        <v>648</v>
       </c>
       <c r="I141" s="15"/>
       <c r="J141" s="16" t="s">
@@ -10148,25 +10166,25 @@
         <v>365</v>
       </c>
       <c r="B142" s="12" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C142" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D142" s="12" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="E142" s="13" t="s">
-        <v>644</v>
+        <v>650</v>
       </c>
       <c r="F142" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G142" s="15" t="s">
-        <v>645</v>
+        <v>651</v>
       </c>
       <c r="H142" s="15" t="s">
-        <v>646</v>
+        <v>652</v>
       </c>
       <c r="I142" s="15"/>
       <c r="J142" s="16" t="s">
@@ -10200,25 +10218,25 @@
         <v>366</v>
       </c>
       <c r="B143" s="12" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C143" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D143" s="12" t="s">
-        <v>647</v>
+        <v>653</v>
       </c>
       <c r="E143" s="13" t="s">
-        <v>648</v>
+        <v>654</v>
       </c>
       <c r="F143" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G143" s="15" t="s">
-        <v>649</v>
+        <v>655</v>
       </c>
       <c r="H143" s="15" t="s">
-        <v>650</v>
+        <v>656</v>
       </c>
       <c r="I143" s="15"/>
       <c r="J143" s="16" t="s">
@@ -10252,25 +10270,25 @@
         <v>367</v>
       </c>
       <c r="B144" s="12" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C144" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D144" s="12" t="s">
-        <v>651</v>
+        <v>657</v>
       </c>
       <c r="E144" s="13" t="s">
-        <v>652</v>
+        <v>658</v>
       </c>
       <c r="F144" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G144" s="15" t="s">
-        <v>653</v>
+        <v>659</v>
       </c>
       <c r="H144" s="15" t="s">
-        <v>654</v>
+        <v>660</v>
       </c>
       <c r="I144" s="15"/>
       <c r="J144" s="16" t="s">
@@ -10310,22 +10328,22 @@
         <v>27</v>
       </c>
       <c r="D145" s="12" t="s">
-        <v>655</v>
+        <v>661</v>
       </c>
       <c r="E145" s="13" t="s">
-        <v>656</v>
+        <v>662</v>
       </c>
       <c r="F145" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G145" s="15" t="s">
-        <v>657</v>
+        <v>663</v>
       </c>
       <c r="H145" s="15" t="s">
-        <v>658</v>
+        <v>664</v>
       </c>
       <c r="I145" s="15" t="s">
-        <v>659</v>
+        <v>665</v>
       </c>
       <c r="J145" s="16" t="s">
         <v>34</v>
@@ -10354,22 +10372,22 @@
         <v>63</v>
       </c>
       <c r="D146" s="12" t="s">
-        <v>660</v>
+        <v>666</v>
       </c>
       <c r="E146" s="13" t="s">
-        <v>661</v>
+        <v>667</v>
       </c>
       <c r="F146" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G146" s="15" t="s">
-        <v>662</v>
+        <v>668</v>
       </c>
       <c r="H146" s="15" t="s">
-        <v>663</v>
+        <v>669</v>
       </c>
       <c r="I146" s="15" t="s">
-        <v>664</v>
+        <v>670</v>
       </c>
       <c r="J146" s="16" t="s">
         <v>34</v>
@@ -10398,22 +10416,22 @@
         <v>59</v>
       </c>
       <c r="D147" s="12" t="s">
-        <v>665</v>
+        <v>671</v>
       </c>
       <c r="E147" s="13" t="s">
-        <v>666</v>
+        <v>672</v>
       </c>
       <c r="F147" s="14" t="s">
         <v>30</v>
       </c>
       <c r="G147" s="15" t="s">
-        <v>667</v>
+        <v>673</v>
       </c>
       <c r="H147" s="15" t="s">
-        <v>668</v>
+        <v>674</v>
       </c>
       <c r="I147" s="15" t="s">
-        <v>669</v>
+        <v>675</v>
       </c>
       <c r="J147" s="16" t="s">
         <v>34</v>
@@ -15208,7 +15226,7 @@
     </row>
     <row r="2" spans="1:6" customHeight="1" ht="14.25">
       <c r="A2" s="2" t="s">
-        <v>670</v>
+        <v>676</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>34</v>
@@ -15216,10 +15234,10 @@
     </row>
     <row r="3" spans="1:6" customHeight="1" ht="14.25">
       <c r="A3" s="2" t="s">
-        <v>671</v>
+        <v>677</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>672</v>
+        <v>678</v>
       </c>
     </row>
     <row r="4" spans="1:6" customHeight="1" ht="14.25">

</xml_diff>